<commit_message>
test cases for registration created
</commit_message>
<xml_diff>
--- a/Open-Cart-Test-Cases.xlsx
+++ b/Open-Cart-Test-Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yathuraj\Desktop\open-cart-manual-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E230E6CC-6160-43C3-A5FC-485AB353EBD7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851B7A11-B0EC-4B89-98FE-C7118EECFAF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1635,8 +1635,8 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -8820,8 +8820,8 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
login test case added
</commit_message>
<xml_diff>
--- a/Open-Cart-Test-Cases.xlsx
+++ b/Open-Cart-Test-Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yathuraj\Desktop\open-cart-manual-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880B6750-5CBC-4390-8562-AED26F247820}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126FF892-647F-4A4F-BC59-BDFDC7A08AF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17066,7 +17066,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>